<commit_message>
Update RouteSchedule with new routes
</commit_message>
<xml_diff>
--- a/RouteSchedule.xlsx
+++ b/RouteSchedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marshallhuckins/Desktop/Desktop - Marshall’s MacBook Air/AMS Routes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F0D8AA-A60C-444E-BDB6-A648F86A5363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB897C0A-8424-D848-B000-02B8D0BDB1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17120" yWindow="700" windowWidth="17080" windowHeight="21440" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7082,7 +7082,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>